<commit_message>
docs(added-BOM): Added Bill of materials
</commit_message>
<xml_diff>
--- a/PS2-PMS-BOM.xlsx
+++ b/PS2-PMS-BOM.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Reference</t>
   </si>
@@ -21,25 +21,163 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>C1</t>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1, C101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1uF, polarised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C size: 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2, C4, C6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7uF 1mOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3, C13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22uF 1mOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C5, C9</t>
   </si>
   <si>
     <t>1uF</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.7uF 1mOhm</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22uF 1mOhm</t>
+    <t xml:space="preserve">C7, C15</t>
+  </si>
+  <si>
+    <t>10uF/6.3V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8, C14</t>
+  </si>
+  <si>
+    <t>0.1uF/6.3V</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>38pF</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>68pF</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>47uF</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>18k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R size: 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2, R7, R14</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>2.2k</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>47k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5, R9, R10</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>590Ohm</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>1.1kOhm</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>80.6k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12, R17, R18, R19</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>10.5k</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>15k</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>5.11Ohm</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>35k</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>55k</t>
   </si>
   <si>
     <t>L1</t>
@@ -54,73 +192,46 @@
     <t>2.0uH</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>18k</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>2.2k</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>47k</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>10kOhm</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>590Ohm</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>1.1kOhm</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>1kOhm</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>C6</t>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>ADP151</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SC174</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>TPS61253</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>bq2407x</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>CSD22202W15</t>
+  </si>
+  <si>
+    <t>BC846</t>
+  </si>
+  <si>
+    <t>BC847C</t>
+  </si>
+  <si>
+    <t>TL431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5pin FPC</t>
   </si>
 </sst>
 </file>
@@ -130,7 +241,7 @@
   <fonts count="5">
     <font>
       <name val="Arial"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <sz val="10.000000"/>
     </font>
     <font>
@@ -172,12 +283,16 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -696,6 +811,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="19.8515625"/>
     <col customWidth="1" min="2" max="2" width="38.140000000000001"/>
     <col customWidth="1" min="3" max="3" width="9"/>
     <col customWidth="1" min="4" max="4" width="24"/>
@@ -724,80 +840,82 @@
       <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
         <v>16</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -807,10 +925,10 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -819,11 +937,11 @@
       <c r="E9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -831,45 +949,50 @@
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11">
+      <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
+      <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
         <v>24</v>
       </c>
+      <c r="B12" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="C12">
         <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -877,10 +1000,10 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -888,21 +1011,21 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -910,10 +1033,10 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -921,19 +1044,213 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
+        <v>39</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
build(pms-board): 2.0 build with cleaner contacts, universal ground, and BOM
</commit_message>
<xml_diff>
--- a/PS2-PMS-BOM.xlsx
+++ b/PS2-PMS-BOM.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Reference</t>
   </si>
@@ -24,6 +24,9 @@
     <t>Qty</t>
   </si>
   <si>
+    <t>Link</t>
+  </si>
+  <si>
     <t xml:space="preserve">C1, C101</t>
   </si>
   <si>
@@ -87,6 +90,9 @@
     <t>47uF</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/kyocera-avx/08056D476MAT2A/13557245</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -186,49 +192,82 @@
     <t xml:space="preserve">1uH 11mOhm</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-dale/IHLP2020CZET1R0M11/9698746</t>
+  </si>
+  <si>
     <t>L2</t>
   </si>
   <si>
     <t>2.0uH</t>
   </si>
   <si>
+    <t>https://www.mouser.com/ProductDetail/KEMET/L8040C2R0NDWDT?qs=e0j0OS9oV9rlkAssOgRULg%3D%3D&amp;countrycode=US&amp;currencycode=USD</t>
+  </si>
+  <si>
     <t>U1</t>
   </si>
   <si>
     <t>ADP151</t>
   </si>
   <si>
+    <t>https://www.mouser.com/ProductDetail/Analog-Devices/ADP151ACPZ-1.8-R7?qs=WIvQP4zGanieq%252BC28QIupQ%3D%3D&amp;countrycode=US&amp;currencycode=USD</t>
+  </si>
+  <si>
     <t>U2</t>
   </si>
   <si>
     <t>SC174</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/semtech-corporation/SC174MLTRT/2342099</t>
+  </si>
+  <si>
     <t>U3</t>
   </si>
   <si>
     <t>TPS61253</t>
   </si>
   <si>
+    <t>https://www.ti.com/product/TPS61253/part-details/TPS61253YFFT</t>
+  </si>
+  <si>
     <t>U4</t>
   </si>
   <si>
     <t>bq2407x</t>
   </si>
   <si>
+    <t>https://www.ti.com/product/BQ24076/part-details/BQ24076RGTR</t>
+  </si>
+  <si>
     <t>U5</t>
   </si>
   <si>
     <t>CSD22202W15</t>
   </si>
   <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CSD22202W15?qs=7GxONfNUZSjRTm5d%2F%252B6xTA%3D%3D&amp;countrycode=US&amp;currencycode=USD</t>
+  </si>
+  <si>
     <t>BC846</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/nexperia-usa-inc/BC846A-215/1232259</t>
+  </si>
+  <si>
     <t>BC847C</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/BC847C-13-F/4471057</t>
+  </si>
+  <si>
     <t>TL431</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/TL431CL3T/2672703</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CSD22202W15?qs=7GxONfNUZSjRTm5d%2F%252B6xTA%3D%3D&amp;gclid=CjwKCAjw7cGUBhA9EiwArBAvota2vhpjwTwy1z6vIuCyxGWTo43K3d8RiZzYXzzM0KivtGQ-qoeiDBoC4FkQAvD_BwE</t>
   </si>
   <si>
     <t xml:space="preserve">5pin FPC</t>
@@ -238,7 +277,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <color theme="1"/>
@@ -262,6 +301,12 @@
       <color rgb="FF1155CC"/>
       <u/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <color theme="10"/>
+      <sz val="10.000000"/>
+      <u/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -283,16 +328,14 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -805,16 +848,18 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
+    <sheetView topLeftCell="B22" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="19.8515625"/>
-    <col customWidth="1" min="2" max="2" width="38.140000000000001"/>
-    <col customWidth="1" min="3" max="3" width="9"/>
-    <col customWidth="1" min="4" max="4" width="24"/>
+    <col customWidth="1" min="2" max="2" width="17.421875"/>
+    <col customWidth="1" min="3" max="3" width="4.8515625"/>
+    <col customWidth="1" min="4" max="4" width="11.140625"/>
+    <col customWidth="1" min="5" max="5" width="80.7109375"/>
+    <col customWidth="1" min="6" max="6" width="17.8515625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -828,29 +873,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -860,10 +907,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
@@ -873,10 +920,10 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -886,10 +933,10 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -899,10 +946,10 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -912,10 +959,10 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -925,10 +972,10 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -938,10 +985,10 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -950,38 +997,40 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>22</v>
+      <c r="A11" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -989,10 +1038,10 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1000,10 +1049,10 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1011,10 +1060,10 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -1022,10 +1071,10 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1033,10 +1082,10 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1044,10 +1093,10 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1055,10 +1104,10 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1066,10 +1115,10 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1077,10 +1126,10 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1088,10 +1137,10 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1099,10 +1148,10 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1110,10 +1159,10 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1121,10 +1170,10 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1132,122 +1181,169 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C27">
         <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
+      <c r="E28" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="C29">
         <v>1</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
+      <c r="E30" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>64</v>
+        <v>69</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C31">
         <v>1</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C32">
         <v>1</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>68</v>
+        <v>75</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="C33">
         <v>1</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
+      <c r="E34" s="6" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C35">
         <v>1</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
+      <c r="E36" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="9" t="s">
-        <v>68</v>
+      <c r="A37" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
+      <c r="E37" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="9" t="s">
-        <v>72</v>
+      <c r="A38" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E11"/>
+    <hyperlink r:id="rId2" ref="E27"/>
+    <hyperlink r:id="rId3" ref="E28"/>
+    <hyperlink r:id="rId4" ref="E29"/>
+    <hyperlink r:id="rId5" ref="E30"/>
+    <hyperlink r:id="rId6" ref="E31"/>
+    <hyperlink r:id="rId7" ref="E32"/>
+    <hyperlink r:id="rId8" ref="E33"/>
+    <hyperlink r:id="rId9" ref="E34"/>
+    <hyperlink r:id="rId10" ref="E35"/>
+    <hyperlink r:id="rId11" ref="E36"/>
+    <hyperlink r:id="rId12" ref="E37"/>
+  </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>